<commit_message>
Removed:  - removed all data that is considered a 'sample' or 'example'  - removed nuget package Added:  - Added extra commentary of what to add and where  - Added a new activity called ERR_DocumentProcessingError where you can write your custom code to handle individual document errors. Changed:  - Sample workflow will be provided seperately
</commit_message>
<xml_diff>
--- a/REFramework_DocumentUnderstanding/VB/Data/Config.xlsx
+++ b/REFramework_DocumentUnderstanding/VB/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\UiPath\DocumentUnderstandingFrameworkTemplate\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\UiPath\GitStudioTemplates\StudioTemplates\REFramework_DocumentUnderstanding\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CC7A83-378A-4288-893C-B4CE75608E54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5016A21E-FF37-4865-993B-17A114BC1E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6315" yWindow="2280" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -334,6 +334,18 @@
   </si>
   <si>
     <t>LogMessage_DataExtractionFinished</t>
+  </si>
+  <si>
+    <t>DocumentUnderstandingQueueName</t>
+  </si>
+  <si>
+    <t>DocumentUnderstandingQueuePath</t>
+  </si>
+  <si>
+    <t>ErrorMessage_DocumentProcessingError</t>
+  </si>
+  <si>
+    <t>A processing error was encountered for document:</t>
   </si>
 </sst>
 </file>
@@ -712,7 +724,7 @@
   <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -915,9 +927,16 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1918,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2223,7 +2242,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>